<commit_message>
DA 16 | Day 4
</commit_message>
<xml_diff>
--- a/Batch/16/Curriculum/Day_4_Logical.xlsx
+++ b/Batch/16/Curriculum/Day_4_Logical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28422"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\15\Curriculum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\16\Curriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E198994-0BA2-421F-9F5F-8C5F75355733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1689FB-58A3-40EC-9C42-098035DA160C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRUE()" sheetId="3" r:id="rId1"/>
@@ -2445,8 +2445,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>74665</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="30" name="Ink 29">
@@ -2465,7 +2465,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="30" name="Ink 29">
@@ -2510,8 +2510,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>151758</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="31" name="Ink 30">
@@ -2530,7 +2530,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="31" name="Ink 30">
@@ -2575,8 +2575,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>162918</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="32" name="Ink 31">
@@ -2595,7 +2595,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="32" name="Ink 31">
@@ -2660,7 +2660,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1456.5">1211 173 4674,'0'0'8463,"-9"-3"-7514,-29-9-279,37 12-628,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 1,0-1 0,-1 1-1,1-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,1 0 0,-1 1-1,0 1 1,-17 41 678,17-41-678,0 0-28,-1-1 0,1 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,1 3 1,-1-4-6,1 0 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,1 0 0,2-1 0,2 1 8,0 0 1,0-1-1,0 0 1,0 0-1,0-1 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 0 1,9-6-1,-13 7-5,0-1-1,0 1 1,1-1-1,-2 0 0,1 0 1,0 0-1,0-1 1,-1 1-1,0 0 1,0-1-1,0 0 0,0 1 1,0-1-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,0-5 1,-1 8-7,0-1 0,1 1 0,-1 0 0,-1-1 1,1 1-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 1,-1 1-1,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,-2 1 0,-3-1-49,1 0-1,-1 0 0,1 1 1,-1-1-1,1 2 1,-11 2-1,15-3-61,0 0 0,0 0 0,0 1 1,1-1-1,-1 0 0,0 1 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,-1 2 0,-3 26-8161,5-24 3306</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1830.47">1491 188 224,'0'0'12062,"-8"8"-10830,8-8-1227,-5 4 141,1 1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 1 0,1 0 0,0 0 0,0 0 0,0 0 1,1 0-1,0 1 0,1-1 0,-1 1 0,1-1 0,-1 10 0,3-14-136,-1-1-1,0 0 1,1 1-1,-1-1 1,0 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,0 1 1,0-1 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,0 0-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1-1 1,1 1-1,-1 0 1,3-2-1,-2 2 31,1 0 0,-1-1 0,1 1-1,-1-1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,0-1 1,0 1 0,1-3-1,-1 2-30,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 1,1 1-1,-1-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0 0 0,0 0 1,0-1-1,0 2 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,-2 1 1,4-2-323,0 1 1,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,8 4-6619</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1922.62">1478 188 5843</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2323.72">1478 188 5843,'138'-105'2606,"-134"103"-2141,0-1 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,2-4 0,-8 16 4214,6 60-4080,3-1 1,18 86-1,-22-145-753,0 0 0,0 0-1,1 1 1,0-1 0,0-1-1,1 1 1,0 0 0,8 10 0,-10-16-98,-1 0 1,1 1 0,0-1 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0 0,1-1-1,-1 1 1,1-1 0,0 0 0,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,0-1 0,0 0-1,0 1 1,-1-1 0,1-1 0,0 1-1,0 0 1,0-1 0,0 1 0,3-2 0,-4 1 46,1-1 1,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0-1,-1 0 1,0 0 0,0 1 0,0-1 0,0 0 0,0-4 0,2-5 368,-1 0 0,0-1 0,0-22 1,-2-1 1615,0 11 2893,-9 24-1782,-25 5-2228,14 7-606,1 1 1,0 1-1,1 1 0,0 1 1,-16 18-1,25-22 377,22-8 87,-1-2-587,176 15-782,-61-13-6380,-94-3 1996</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2323.71">1478 188 5843,'138'-105'2606,"-134"103"-2141,0-1 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,2-4 0,-8 16 4214,6 60-4080,3-1 1,18 86-1,-22-145-753,0 0 0,0 0-1,1 1 1,0-1 0,0-1-1,1 1 1,0 0 0,8 10 0,-10-16-98,-1 0 1,1 1 0,0-1 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0 0,1-1-1,-1 1 1,1-1 0,0 0 0,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,0-1 0,0 0-1,0 1 1,-1-1 0,1-1 0,0 1-1,0 0 1,0-1 0,0 1 0,3-2 0,-4 1 46,1-1 1,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0-1,-1 0 1,0 0 0,0 1 0,0-1 0,0 0 0,0-4 0,2-5 368,-1 0 0,0-1 0,0-22 1,-2-1 1615,0 11 2893,-9 24-1782,-25 5-2228,14 7-606,1 1 1,0 1-1,1 1 0,0 1 1,-16 18-1,25-22 377,22-8 87,-1-2-587,176 15-782,-61-13-6380,-94-3 1996</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2654.1">2144 219 6259,'0'0'8561,"34"55"-6760,-30-51-1750,0 0-1,1 0 1,0-1 0,0 1 0,0-1 0,0 0-1,0-1 1,1 1 0,-1-1 0,1 0-1,-1 0 1,1-1 0,0 0 0,7 1-1,-10-1 0,0-1-1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1-1 0,-1 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 1,1-1-1,0 1 0,-1-1 0,0 0 0,1 0 1,-1 0-1,0-1 0,0 1 0,0 0 0,0-1 0,1-3 1,0-1 101,0 0 1,-1 0 0,-1 0 0,1 0 0,-1-1-1,0 1 1,-1-1 0,0-7 0,0 13-194,0 1 1,0-1 0,0 0-1,0 0 1,-1 1-1,1-1 1,0 0 0,-1 0-1,0 1 1,1-1-1,-1 0 1,0 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0 0 0,0-1-1,-1 1 1,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1 1-1,-1-1 1,0 0 0,0 1-1,1 0 1,-1-1-1,0 1 1,0 0 0,-2 0-1,3 9-5835,1-3 1131</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2906.65">2478 22 1153,'0'0'15084,"0"-6"-14132,0-9-717,2 23 16,3 46 351,-1-5 130,16 339 367,-19-222-7411,6-170-1327,8-22 2939</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3141.53">2571 452 2673,'0'-19'2014,"-1"-13"-1348,0-11 1242,3-45 0,-2 79-1513,1-1 0,0 1 0,1-1 0,0 1 1,0 0-1,1 0 0,0 0 0,1 0 0,0 0 0,0 1 0,9-13 0,-9 17-288,-1 1-1,1-1 0,0 1 0,0 0 0,0 1 1,1-1-1,-1 1 0,1-1 0,-1 1 1,1 0-1,0 1 0,0-1 0,6 0 1,66-3 1331,-72 5-1309,-4 0-93,0 0-1,1 0 1,-1 0-1,0 0 0,0 1 1,1-1-1,-1 0 1,0 1-1,0-1 1,0 1-1,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,-1 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,0 1-1,0-1 1,-1 2-1,1 0 43,0 1-1,-1-1 0,1 1 1,-1-1-1,0 0 1,0 1-1,-1-1 0,1 0 1,0 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,-2 2-1,-8 5 43,1-1 0,-1-1-1,-1 0 1,0-1 0,0 0 0,-23 8 0,-88 22-2301,85-30-1186,-3-6-2825</inkml:trace>
@@ -2694,7 +2694,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">43 174 2209,'0'0'10133,"0"13"-9498,1 38 787,-2 73 340,0-112-1687,0 0 0,-1 0 1,-1 0-1,0 0 0,-1-1 0,0 1 0,-10 20 0,14-32-72,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,-4-23-49,3-28-157,1 50 203,0-19-162,1-1 1,1 0-1,1 0 1,1 0 0,0 1-1,2 0 1,0 0-1,2 0 1,13-26 0,-20 44 162,-1 1 0,1-1 0,0 0 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 1 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1 0 1,0 0-1,-1 0 0,1 1 0,0-1 1,0 0-1,-1 1 0,1-1 1,0 1-1,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,-1 0 1,1-1-1,0 1 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 1 0,1 2 1,8 5 121,-1 2 1,0-1 0,-1 1 0,11 17 0,-20-28-121,11 16-74,-1 1 0,-1 0-1,-1 0 1,-1 1 0,0 0 0,-1 0 0,4 21-1,-2 33-7036,-8-52 833</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="202.57">52 349 4306,'0'0'7187,"37"-62"-7251,-4 53-112,4 3-512,-10 3-465,5 0-607,-15 3-754,4 0-127</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="525.52">321 244 1809,'0'0'10650,"2"3"-10322,5 6 41,-1 1 0,0 0 0,-1-1-1,8 21 1,-10-21-272,0 0-1,1-1 1,0 0-1,0 0 1,1 0-1,0 0 1,1-1-1,-1 0 1,1 0-1,13 11 1,-18-16-75,1-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,1 0-1,-1-1 0,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,4 0-1,-5 0 26,0-1-1,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,0-2 0,2-6 249,0 0-1,-1 0 1,-1 0-1,1-1 1,-1-16 0,3-5-623,-4 29 198,0 1-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,0 0 0,1 1-1,-1 0 1,0-1 0,0 1-1,1-1 1,35 0-6269,-21 2 5143,15-1-2200</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1074.35">839 265 688,'0'0'10282,"-17"-8"-8958,-55-25-81,70 32-1204,-1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 1 0,-1-1 1,1 1-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 1 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1 0 1,1 0-1,0 1 0,-1-1 1,1 0-1,0 1 0,0-1 1,1 1-1,-1-1 0,-2 7 1,1-3-26,0 1 0,0 0 1,1 0-1,0 0 0,1 0 1,-1 1-1,2-1 1,-1 0-1,1 1 0,0-1 1,0 0-1,3 14 0,-3-20-25,1 1 0,-1-1 0,1 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,3 0 0,-1 1-8,0-1 0,1 0 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,3-3 1,-2 1 42,0 0 0,0 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,2-8 0,-4 12 62,1 3-88,1-1 1,0 1-1,-1 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 3 0,8 15 28,-8-17-52,1 0 0,0-1 0,0 1-1,0 0 1,0-1 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,0-1-1,0 0 1,0 0 0,-1 0 0,7 0-1,-8-1-35,1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 0 0,0 0 0,0 1 0,0-1 0,-1-1 0,1 1 1,0 0-1,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 1,0 0-1,3-4 0,-2 0-23,1 1 1,-1-1-1,0 0 0,0 0 1,-1-1-1,0 1 1,0 0-1,0-1 0,-1 1 1,0-1-1,0 0 1,-1-13 650,0 38-271,0 3-67,-1-8-120,1 0 0,0 0 1,1 0-1,5 23 0,-6-33-128,1 0 1,0-1 0,0 1-1,0-1 1,0 1-1,0-1 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,4-1-1,-3 0-117,4 1-574,-1-1 0,1 0 0,0 0 0,-1-1 0,11-1-1,10-11-4803</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1074.34">839 265 688,'0'0'10282,"-17"-8"-8958,-55-25-81,70 32-1204,-1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 1 0,-1-1 1,1 1-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 1 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1 0 1,1 0-1,0 1 0,-1-1 1,1 0-1,0 1 0,0-1 1,1 1-1,-1-1 0,-2 7 1,1-3-26,0 1 0,0 0 1,1 0-1,0 0 0,1 0 1,-1 1-1,2-1 1,-1 0-1,1 1 0,0-1 1,0 0-1,3 14 0,-3-20-25,1 1 0,-1-1 0,1 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,3 0 0,-1 1-8,0-1 0,1 0 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,3-3 1,-2 1 42,0 0 0,0 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,2-8 0,-4 12 62,1 3-88,1-1 1,0 1-1,-1 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 3 0,8 15 28,-8-17-52,1 0 0,0-1 0,0 1-1,0 0 1,0-1 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,0-1-1,0 0 1,0 0 0,-1 0 0,7 0-1,-8-1-35,1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 0 0,0 0 0,0 1 0,0-1 0,-1-1 0,1 1 1,0 0-1,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 1,0 0-1,3-4 0,-2 0-23,1 1 1,-1-1-1,0 0 0,0 0 1,-1-1-1,0 1 1,0 0-1,0-1 0,-1 1 1,0-1-1,0 0 1,-1-13 650,0 38-271,0 3-67,-1-8-120,1 0 0,0 0 1,1 0-1,5 23 0,-6-33-128,1 0 1,0-1 0,0 1-1,0-1 1,0 1-1,0-1 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,4-1-1,-3 0-117,4 1-574,-1-1 0,1 0 0,0 0 0,-1-1 0,11-1-1,10-11-4803</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1215.82">1057 65 3025,'0'0'1041</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1440.08">1057 78 7027,'119'-21'5715,"-119"30"-5203,0 19-96,0 9 673,5 2-673,0 5-176,6-5-176,0 4-48,0-3-16,5 0-928,5-3-1137,6-9-817,5-10 225,6-12 1072</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2179.36">1662 293 1713,'0'0'10485,"-12"-11"-9066,-40-36-440,49 45-918,0 0 0,0 0 0,-1 0 0,1 1 0,0 0 1,-1-1-1,1 1 0,-1 1 0,1-1 0,-1 0 0,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 1,0-1-1,1 1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 1 0,-4 3 0,0 0 12,0 1 0,1 0-1,-1 0 1,1 1-1,1-1 1,-1 2-1,-8 12 1,13-17-72,0 0 0,1 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,0 1 0,1-1-1,-1 1 1,1-1 0,0 1 0,0-1 0,0 5-1,0-4-22,1-3-35,0 0 0,-1 0 0,1 0 0,0 0 0,0-1-1,0 1 1,-1 0 0,1-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,1-1-1,-1 1 1,1 0 0,35-2-982,-32 1 980,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,3-4 0,21-14 49,-28 21 656,11 40 413,-10-36-1038,0 1 1,1-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,1-1-1,-1 1 0,1-1 1,0 0-1,0 0 1,0-1-1,9 5 1,-11-6-13,0 0 1,1 0 0,-1-1-1,1 1 1,-1-1 0,0 1-1,1-1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,-1 0-1,1 0 1,2-3 0,2-6 6,0 0 1,0 0-1,-1-1 1,-1 0 0,0 0-1,0 0 1,-1 0 0,-1 0-1,2-16 1,0-85 1119,-4 105-590,-2 56-570,1-29 36,0 0-1,1 0 0,5 37 1,-4-54-26,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,2 0 0,52 1-504,-39-2 367,4 1-20,-14-1 29,1 0 0,0 1 0,0 1 0,-1-1-1,1 1 1,0 0 0,-1 1 0,1 0 0,-1 0 0,12 6 0,-18-8 138,-1 0-1,0 0 1,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,1 0 1,-1 0-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 0 1,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 0 1,-1 0-1,0 1 1,-23 9 346,21-9-335,-124 32 807,37-11-1585,88-22-939,2-9-7761</inkml:trace>
@@ -2730,7 +2730,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">19 298 1953,'0'0'7297,"-5"-2"-6609,-9-9 247,21 7 1108,36 7 900,-26-1-3792,402 23 1190,-349-19-418,-70-8 85,0 0 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 0 1,-1 1-1,0-1 1,1 1-1,-3-3 1,-1 0 2,0 0 1,0 0-1,-1 1 0,1-1 1,-1 1-1,0 0 1,0 0-1,0 1 0,-1 0 1,-9-4-1,72 1-1502,-50 5 1462,0 0 0,0 0 0,0 1 0,-1 0 0,1 0-1,10 4 1,-16-5 28,0 1-1,-1-1 1,1 0-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 1-1,0 0 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 1-1,-1-1 21,-1 1 0,1 0-1,0 0 1,-1-1 0,1 1-1,-1 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,-2 2 0,-35 32 196,32-30-194,-1 0 0,1 0 0,0 1 0,1 0 0,-10 13 0,13-16-452,0 0 0,1 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,1 1 0,-1-1 1,1 1-1,-1 6 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="561.79">895 191 3185,'0'0'5921,"1"4"-4313,4 38-657,-2-1 0,-5 64 0,1-30-1512,1-74 62,1-7-547,4-57 34,-6 54 1026,1 1 0,0 0 0,1-1-1,-1 1 1,2 0 0,-1-1 0,1 1 0,0 0 0,1 0-1,0 0 1,0 1 0,7-13 0,-8 19 16,1-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 1 0,0 0 1,0 0-1,-1 0 0,6 1 0,38 6 615,-36-2-511,-1 1 1,-1 0-1,1 0 0,-1 0 0,0 1 0,-1 1 0,0-1 0,0 1 0,0 0 0,7 12 0,-6-7-723,2-1-1,-1-1 1,22 19-1,-30-29 276,1 0-1,-1 0 1,1 0 0,0 0-1,-1-1 1,1 1-1,-1-1 1,1 1-1,0-1 1,0 1 0,-1-1-1,1 0 1,2 0-1,2 0-2299</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="832.67">1242 255 560,'0'0'3877,"0"-17"-2685,0-54 38,-2 110 4151,-2 102-5354,4-139-304,1 1 1,-1-1-1,0 0 0,1 1 0,-1-1 1,1 0-1,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 1 1,0-1-1,4 2 0,10 2-3519</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1177.84">1242 255 1393,'125'2'1827,"-106"-4"513,-20 0-881,0 1-1385,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 1,0 0-1,-2 3 1,1-1 1,1 1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0 0,0 1 0,1 3-1,-2-5-64,1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,0 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,1 0 0,3 0 0,-4 0-1,1 0-1,-1 1 1,1-1 0,-1-1 0,1 1 0,0 0 0,-1-1-1,0 1 1,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,0 1 0,2-2 0,-3-1 93,1 1 1,0 0-1,-1-1 0,0 1 1,0-1-1,0 1 1,0-1-1,-1 0 1,0 1-1,1-1 1,-1 0-1,-1-5 1,1 8-65,-1-1-1,1 1 1,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,0-1-1,-1 1 1,1 0 0,-1-1 0,1 1 0,-4 0 0,-43-3-1159,47 3 971,-1 0-1505</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1177.83">1242 255 1393,'125'2'1827,"-106"-4"513,-20 0-881,0 1-1385,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 1,0 0-1,-2 3 1,1-1 1,1 1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0 0,0 1 0,1 3-1,-2-5-64,1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,0 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,1 0 0,3 0 0,-4 0-1,1 0-1,-1 1 1,1-1 0,-1-1 0,1 1 0,0 0 0,-1-1-1,0 1 1,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,0 1 0,2-2 0,-3-1 93,1 1 1,0 0-1,-1-1 0,0 1 1,0-1-1,0 1 1,0-1-1,-1 0 1,0 1-1,1-1 1,-1 0-1,-1-5 1,1 8-65,-1-1-1,1 1 1,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,0-1-1,-1 1 1,1 0 0,-1-1 0,1 1 0,-4 0 0,-43-3-1159,47 3 971,-1 0-1505</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1463.77">1640 0 2817,'0'0'4450,"-6"20"-3497,-2 14-392,1 1 0,2 0 0,-1 49-1,5-72-410,1 0-27,0 0-1,0 0 1,1 0 0,1 0-1,0 0 1,3 11 0,-3-19-115,0 0 1,0 0 0,0 0-1,1-1 1,-1 1 0,1 0-1,0-1 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,1-1 1,0 1-1,0-1 1,-1 0 0,2 0-1,-1-1 1,0 1 0,5 0-1,3 1-822,1-1-1,-1 0 0,1-1 0,15-1 0,-22-1-1572,-5-7-548</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1603.37">1645 326 2273,'0'0'9060,"-11"-15"-9156,44 9 16,10-3-512,10 3-737,1-4-1408,0 1-1361</inkml:trace>
 </inkml:ink>
@@ -34084,8 +34084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9565CD32-2EAF-4F59-96F0-F38C63E9D7F0}">
   <dimension ref="B2:B282"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B282"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="R66" sqref="R66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -39543,8 +39543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:D1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C9"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -40651,8 +40651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:M1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -41982,8 +41982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -43136,8 +43136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>